<commit_message>
xlsx created for experimental purpose.
</commit_message>
<xml_diff>
--- a/2η εργασία/DiceCoefOutput1.xlsx
+++ b/2η εργασία/DiceCoefOutput1.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marios\Documents\GitHub\2η εργασία\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="48">
   <si>
     <t>ISBN</t>
   </si>
@@ -37,134 +42,134 @@
     <t>DiceCoefScores</t>
   </si>
   <si>
-    <t>1400031346</t>
-  </si>
-  <si>
-    <t>037542217X</t>
-  </si>
-  <si>
-    <t>0375422188</t>
-  </si>
-  <si>
-    <t>0385334621</t>
-  </si>
-  <si>
-    <t>0440241537</t>
-  </si>
-  <si>
-    <t>0375503943</t>
-  </si>
-  <si>
-    <t>0440242002</t>
-  </si>
-  <si>
-    <t>3485008702</t>
-  </si>
-  <si>
-    <t>038550120X</t>
-  </si>
-  <si>
-    <t>1400031362</t>
-  </si>
-  <si>
-    <t>The No. 1 Ladies' Detective Agency</t>
-  </si>
-  <si>
-    <t>The Kalahari Typing School for Men : More from the No. 1 Ladies' Detective Agency</t>
-  </si>
-  <si>
-    <t>The Full Cupboard of Life: More from the No. 1 Ladies' Detective Agency</t>
-  </si>
-  <si>
-    <t>The Greatest Generation</t>
-  </si>
-  <si>
-    <t>The King of Torts</t>
-  </si>
-  <si>
-    <t>The Greatest Generation Speaks : Letters and Reflections</t>
-  </si>
-  <si>
-    <t>Bleachers</t>
-  </si>
-  <si>
-    <t>Ein Krokodil fÃ?Â¼r Mma Ramotswe. Der erste Fall der 'No. 1 Ladies Detektive Agency'.</t>
-  </si>
-  <si>
-    <t>A Painted House</t>
-  </si>
-  <si>
-    <t>Morality for Beautiful Girls (No.1 Ladies Detective Agency)</t>
-  </si>
-  <si>
-    <t>Alexander McCall Smith</t>
-  </si>
-  <si>
-    <t>TOM BROKAW</t>
-  </si>
-  <si>
-    <t>JOHN GRISHAM</t>
-  </si>
-  <si>
-    <t>Anchor (UK)</t>
-  </si>
-  <si>
-    <t>Pantheon</t>
-  </si>
-  <si>
-    <t>Delta</t>
-  </si>
-  <si>
-    <t>Dell</t>
-  </si>
-  <si>
-    <t>Random House</t>
-  </si>
-  <si>
-    <t>Nymphenburger</t>
-  </si>
-  <si>
-    <t>Doubleday</t>
-  </si>
-  <si>
-    <t>Anchor</t>
-  </si>
-  <si>
-    <t>['detective agency', '1 ladies']</t>
-  </si>
-  <si>
-    <t>['kalahari typing school', 'detective agency', '1 ladies', 'men']</t>
-  </si>
-  <si>
-    <t>['full cupboard', 'detective agency', '1 ladies', 'life']</t>
-  </si>
-  <si>
-    <t>['greatest generation']</t>
-  </si>
-  <si>
-    <t>['torts', 'king']</t>
-  </si>
-  <si>
-    <t>['greatest generation speaks', 'reflections', 'letters']</t>
-  </si>
-  <si>
-    <t>['bleachers']</t>
-  </si>
-  <si>
-    <t>["1 ladies detektive agency '.", 'der erste fall der', 'â¼r mma ramotswe', 'ein krokodil fã']</t>
-  </si>
-  <si>
-    <t>['painted house']</t>
-  </si>
-  <si>
-    <t>['1 ladies detective agency', 'beautiful girls', 'morality']</t>
+    <t>0451408977</t>
+  </si>
+  <si>
+    <t>0451409361</t>
+  </si>
+  <si>
+    <t>0451410556</t>
+  </si>
+  <si>
+    <t>0670888702</t>
+  </si>
+  <si>
+    <t>0451410386</t>
+  </si>
+  <si>
+    <t>067003004X</t>
+  </si>
+  <si>
+    <t>080505622X</t>
+  </si>
+  <si>
+    <t>0345394259</t>
+  </si>
+  <si>
+    <t>0440167477</t>
+  </si>
+  <si>
+    <t>0345387554</t>
+  </si>
+  <si>
+    <t>The Stargazey: A Richard Jury Mystery (Richard Jury Mysteries (Paperback))</t>
+  </si>
+  <si>
+    <t>The Lamorna Wink: A Richard Jury Mystery (Richard Jury Mysteries (Paperback))</t>
+  </si>
+  <si>
+    <t>The Blue Last: A Richard Jury Mystery (Richard Jury Mysteries (Paperback))</t>
+  </si>
+  <si>
+    <t>The Lamorna Wink: A Richard Jury Mystery (Richard Jury Mysteries (Hardcover))</t>
+  </si>
+  <si>
+    <t>The Five Bells and Bladebone (Richard Jury Mysteries (Paperback))</t>
+  </si>
+  <si>
+    <t>The Blue Last: A Richard Jury Mystery</t>
+  </si>
+  <si>
+    <t>The Stargazey (Richard Jury Mystery Series/Martha Grimes)</t>
+  </si>
+  <si>
+    <t>Hotel Paradise</t>
+  </si>
+  <si>
+    <t>The Old Fox Deceiv'D</t>
+  </si>
+  <si>
+    <t>The Horse You Came In On</t>
+  </si>
+  <si>
+    <t>Martha Grimes</t>
+  </si>
+  <si>
+    <t>Anne Cameron</t>
+  </si>
+  <si>
+    <t>DANIEL QUINN</t>
+  </si>
+  <si>
+    <t>Onyx Books</t>
+  </si>
+  <si>
+    <t>Viking Books</t>
+  </si>
+  <si>
+    <t>Henry Holt &amp;amp; Company</t>
+  </si>
+  <si>
+    <t>Ballantine Books</t>
+  </si>
+  <si>
+    <t>Dell Publishing Company</t>
+  </si>
+  <si>
+    <t>['richard jury mystery', 'richard jury mysteries', 'paperback ))', 'stargazey']</t>
+  </si>
+  <si>
+    <t>['richard jury mystery', 'richard jury mysteries', 'paperback ))', 'lamorna wink']</t>
+  </si>
+  <si>
+    <t>['richard jury mystery', 'richard jury mysteries', 'paperback ))', 'blue last']</t>
+  </si>
+  <si>
+    <t>['richard jury mystery', 'richard jury mysteries', 'lamorna wink', 'hardcover ))']</t>
+  </si>
+  <si>
+    <t>['richard jury mysteries', 'paperback ))', 'five bells', 'bladebone']</t>
+  </si>
+  <si>
+    <t>['richard jury mystery', 'blue last']</t>
+  </si>
+  <si>
+    <t>['richard jury mystery series', 'martha grimes', 'stargazey']</t>
+  </si>
+  <si>
+    <t>['hotel paradise']</t>
+  </si>
+  <si>
+    <t>['old fox deceiv']</t>
+  </si>
+  <si>
+    <t>['horse', 'came']</t>
+  </si>
+  <si>
+    <t>['richard jury mystery', 'richard jury mysteries', 'paperback ))', 'case', 'altered']</t>
+  </si>
+  <si>
+    <t>['copper woman', 'daughters']</t>
+  </si>
+  <si>
+    <t>['story', 'b']</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -227,6 +232,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -273,7 +286,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -305,9 +318,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -339,6 +353,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -514,14 +529,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="72.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="70.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -544,9 +571,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>3318</v>
+        <v>15333</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
@@ -558,21 +585,21 @@
         <v>27</v>
       </c>
       <c r="E2">
-        <v>2002</v>
+        <v>1999</v>
       </c>
       <c r="F2" t="s">
         <v>30</v>
       </c>
       <c r="G2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="H2">
-        <v>0.7499002493765585</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
+        <v>0.73066948014578936</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>954</v>
+        <v>8216</v>
       </c>
       <c r="B3" t="s">
         <v>8</v>
@@ -584,21 +611,21 @@
         <v>27</v>
       </c>
       <c r="E3">
-        <v>2003</v>
+        <v>2000</v>
       </c>
       <c r="F3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="H3">
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
+        <v>0.730569729522348</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>10850</v>
+        <v>285</v>
       </c>
       <c r="B4" t="s">
         <v>9</v>
@@ -610,21 +637,21 @@
         <v>27</v>
       </c>
       <c r="E4">
-        <v>2004</v>
+        <v>2002</v>
       </c>
       <c r="F4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="H4">
-        <v>0.6999002493765587</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
+        <v>0.73037022827546516</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>11992</v>
+        <v>11997</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
@@ -633,24 +660,24 @@
         <v>20</v>
       </c>
       <c r="D5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E5">
-        <v>2001</v>
+        <v>1999</v>
       </c>
       <c r="F5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="H5">
-        <v>0.6427573922337015</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
+        <v>0.65374640322271249</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>1474</v>
+        <v>11945</v>
       </c>
       <c r="B6" t="s">
         <v>11</v>
@@ -659,24 +686,24 @@
         <v>21</v>
       </c>
       <c r="D6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E6">
-        <v>2003</v>
+        <v>2002</v>
       </c>
       <c r="F6" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="G6" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="H6">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
+        <v>0.65344715135238829</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>13036</v>
+        <v>16110</v>
       </c>
       <c r="B7" t="s">
         <v>12</v>
@@ -685,24 +712,24 @@
         <v>22</v>
       </c>
       <c r="D7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E7">
-        <v>1999</v>
+        <v>2001</v>
       </c>
       <c r="F7" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G7" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="H7">
-        <v>0.4999002493765586</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
+        <v>0.59060983903876674</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>11924</v>
+        <v>11132</v>
       </c>
       <c r="B8" t="s">
         <v>13</v>
@@ -711,24 +738,24 @@
         <v>23</v>
       </c>
       <c r="D8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E8">
-        <v>2004</v>
+        <v>1998</v>
       </c>
       <c r="F8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G8" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="H8">
-        <v>0.4999002493765586</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>5163</v>
+        <v>10119</v>
       </c>
       <c r="B9" t="s">
         <v>14</v>
@@ -740,21 +767,21 @@
         <v>27</v>
       </c>
       <c r="E9">
-        <v>2001</v>
+        <v>1997</v>
       </c>
       <c r="F9" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G9" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="H9">
-        <v>0.4999002493765586</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>4210</v>
+        <v>9623</v>
       </c>
       <c r="B10" t="s">
         <v>15</v>
@@ -763,24 +790,24 @@
         <v>25</v>
       </c>
       <c r="D10" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E10">
-        <v>2001</v>
+        <v>1988</v>
       </c>
       <c r="F10" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G10" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="H10">
-        <v>0.4999002493765586</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>3158</v>
+        <v>9988</v>
       </c>
       <c r="B11" t="s">
         <v>16</v>
@@ -792,16 +819,58 @@
         <v>27</v>
       </c>
       <c r="E11">
-        <v>2002</v>
+        <v>1996</v>
       </c>
       <c r="F11" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="G11" t="s">
+        <v>44</v>
+      </c>
+      <c r="H11">
+        <v>0.49990024937655858</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>0</v>
+      </c>
+      <c r="D12" t="s">
+        <v>27</v>
+      </c>
+      <c r="E12">
+        <v>1998</v>
+      </c>
+      <c r="G12" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>1</v>
+      </c>
+      <c r="D13" t="s">
+        <v>28</v>
+      </c>
+      <c r="E13">
+        <v>1988</v>
+      </c>
+      <c r="G13" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>2</v>
+      </c>
+      <c r="D14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E14">
+        <v>1997</v>
+      </c>
+      <c r="G14" t="s">
         <v>47</v>
-      </c>
-      <c r="H11">
-        <v>0.4999002493765586</v>
       </c>
     </row>
   </sheetData>

</xml_diff>